<commit_message>
gtpw graph algorithm first commit
</commit_message>
<xml_diff>
--- a/programDocSample.xlsx
+++ b/programDocSample.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nirvik Saha\Documents\NetBeansProjects\ApachePoiSwingDemo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nirvik Saha\Documents\NetBeansProjects\GTPW_graph\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>PROGRAM ID</t>
   </si>
@@ -114,14 +114,47 @@
     <t>Staff Respite Room</t>
   </si>
   <si>
-    <t>blank</t>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>0,3</t>
+  </si>
+  <si>
+    <t>9,8,11</t>
+  </si>
+  <si>
+    <t>7,8</t>
+  </si>
+  <si>
+    <t>10,5,9</t>
+  </si>
+  <si>
+    <t>9,8</t>
+  </si>
+  <si>
+    <t>3,2</t>
+  </si>
+  <si>
+    <t>8,9,5</t>
+  </si>
+  <si>
+    <t>10,8,4</t>
+  </si>
+  <si>
+    <t>2,5,3</t>
+  </si>
+  <si>
+    <t>3,4,5,6</t>
+  </si>
+  <si>
+    <t>4,1,0,5,6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -252,6 +285,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -598,8 +637,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -957,11 +997,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="23" customWidth="1"/>
+    <col min="7" max="7" width="17.5546875" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -1023,6 +1068,9 @@
       <c r="H2" t="s">
         <v>13</v>
       </c>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
       <c r="J2">
         <v>0</v>
       </c>
@@ -1055,6 +1103,9 @@
       <c r="H3" t="s">
         <v>13</v>
       </c>
+      <c r="I3" t="s">
+        <v>32</v>
+      </c>
       <c r="J3">
         <v>0</v>
       </c>
@@ -1087,6 +1138,9 @@
       <c r="H4" t="s">
         <v>17</v>
       </c>
+      <c r="I4" t="s">
+        <v>41</v>
+      </c>
       <c r="J4">
         <v>1</v>
       </c>
@@ -1095,7 +1149,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
@@ -1119,6 +1173,9 @@
       <c r="H5" t="s">
         <v>17</v>
       </c>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
       <c r="J5">
         <v>2</v>
       </c>
@@ -1127,7 +1184,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
@@ -1151,6 +1208,9 @@
       <c r="H6" t="s">
         <v>22</v>
       </c>
+      <c r="I6" t="s">
+        <v>40</v>
+      </c>
       <c r="J6">
         <v>3</v>
       </c>
@@ -1159,7 +1219,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7">
+      <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
@@ -1182,6 +1242,9 @@
       </c>
       <c r="H7" t="s">
         <v>22</v>
+      </c>
+      <c r="I7" t="s">
+        <v>39</v>
       </c>
       <c r="J7">
         <v>3</v>
@@ -1212,6 +1275,9 @@
       <c r="H8" t="s">
         <v>22</v>
       </c>
+      <c r="I8" t="s">
+        <v>37</v>
+      </c>
       <c r="J8">
         <v>3</v>
       </c>
@@ -1241,6 +1307,9 @@
       <c r="H9" t="s">
         <v>22</v>
       </c>
+      <c r="I9" t="s">
+        <v>36</v>
+      </c>
       <c r="J9">
         <v>3</v>
       </c>
@@ -1270,6 +1339,9 @@
       <c r="H10" t="s">
         <v>22</v>
       </c>
+      <c r="I10" t="s">
+        <v>35</v>
+      </c>
       <c r="J10">
         <v>4</v>
       </c>
@@ -1302,6 +1374,9 @@
       <c r="H11" t="s">
         <v>22</v>
       </c>
+      <c r="I11" t="s">
+        <v>34</v>
+      </c>
       <c r="J11">
         <v>4</v>
       </c>
@@ -1331,6 +1406,9 @@
       <c r="H12" t="s">
         <v>22</v>
       </c>
+      <c r="I12" t="s">
+        <v>33</v>
+      </c>
       <c r="J12">
         <v>4</v>
       </c>
@@ -1360,14 +1438,15 @@
       <c r="H13" t="s">
         <v>22</v>
       </c>
+      <c r="I13" t="s">
+        <v>38</v>
+      </c>
       <c r="J13">
         <v>4</v>
-      </c>
-      <c r="K13" t="s">
-        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>